<commit_message>
Delete patient profile (#34)
* propal w/o patient profile

* rm  cds patient

* add cano

* rm cds patient

* Update interaction_transaction.md

* Update interaction_restful.md 9dd109c205af89a4bfea19bda82ceb88a7beea69
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-cds-bundle-response-recherche.xlsx
+++ b/main/ig/StructureDefinition-cds-bundle-response-recherche.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-28T14:08:32+00:00</t>
+    <t>2024-05-31T13:43:47+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -992,7 +992,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Patient {http://interop.esante.gouv.fr/ig/fhir/cds/StructureDefinition/cds-fr-patient}
+    <t xml:space="preserve">Patient {https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-patient}
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
prepare release 2.0.0-ballot (#36) 12f3ae73abcb5f0bc997e099c076428c143191a3
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-cds-bundle-response-recherche.xlsx
+++ b/main/ig/StructureDefinition-cds-bundle-response-recherche.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>2.0.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-31T13:43:47+00:00</t>
+    <t>2024-06-25T20:35:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Mise-à-jour des diagrammes de création/mise-à-jour de Cercle de Soins en mode Transactions. (#47)
* Update creation and update of CareTeam using PlantUML

* Use the plantuml diagrams in the interaction_transaction page

* Remove old png files 18cf332fd4e0fffda4d7fbb50e033afa6eb73ed8
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-cds-bundle-response-recherche.xlsx
+++ b/main/ig/StructureDefinition-cds-bundle-response-recherche.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-24T16:16:30+00:00</t>
+    <t>2025-11-17T08:43:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -361,7 +361,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -1873,17 +1873,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="57.6875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="19.109375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="28.78515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="49.45703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.3828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="24.67578125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="95.953125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="82.26171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1892,26 +1892,26 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="168.19140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="49.01171875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.98046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="144.1953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="42.01953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="29.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="31.1328125" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="50.96875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="42.9765625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="26.69140625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="43.6953125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="36.84375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
mise à jour des dépendances (#45) a8408d77ae7c614f6e556d3de9f058285ae0e198
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-cds-bundle-response-recherche.xlsx
+++ b/main/ig/StructureDefinition-cds-bundle-response-recherche.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-17T08:43:36+00:00</t>
+    <t>2025-11-17T09:24:16+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1462,10 +1462,10 @@
 </t>
   </si>
   <si>
-    <t>A person with a  formal responsibility in the provisioning of healthcare or related services | Prestataire de santé</t>
-  </si>
-  <si>
-    <t>A person who is directly or indirectly involved in the provisioning of healthcare | Un professionnel impliqué directement ou indirectement dans la prise en charge d'une personne.</t>
+    <t>A person with a  formal responsibility in the provisioning of healthcare or related services</t>
+  </si>
+  <si>
+    <t>A person who is directly or indirectly involved in the provisioning of healthcare.</t>
   </si>
   <si>
     <t>Bundle.entry:practitionerPro.search</t>

</xml_diff>